<commit_message>
feat: finalizando ejercicio 1 lab 7
</commit_message>
<xml_diff>
--- a/labs/lab7/lab7.xlsx
+++ b/labs/lab7/lab7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UVG GitHub Repositorios\2025\Inteligencia Artificial\labs\lab7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6908E258-4DD2-40E0-A0F2-061661B40F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435D3F48-96ED-45CC-ADC4-8844F4224476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8F1ECDA0-F4DF-3946-9953-220E6ED439C0}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
   <si>
     <t>Se tienen tres cajas, cada una conteniendo 100 cartas:</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Se elige una de las cajas al azar, y luego se elige una carta dentro de la caja</t>
   </si>
   <si>
-    <t>¿Cuál es la probabilidad de elegir una carta roja?</t>
-  </si>
-  <si>
     <t>enfermedad?</t>
   </si>
   <si>
@@ -154,20 +151,124 @@
     <t>Independientes, P(X) con valores distintos, P(Y) con valores distintos</t>
   </si>
   <si>
-    <t>La caja Naranja contiene 55 cartas rojas, y 45 cartas azules.</t>
-  </si>
-  <si>
-    <t>La caja Amarilla contiene 75 cartas rojas, y 25 cartas azules.</t>
-  </si>
-  <si>
-    <t>La caja Verde contiene 60 cartas rojas, y 40 cartas azules.</t>
+    <t xml:space="preserve">cantidada de cajas </t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>cartas en cada cada caja individual</t>
+  </si>
+  <si>
+    <t>Datos generales:</t>
+  </si>
+  <si>
+    <t>Datos caja amarilla:</t>
+  </si>
+  <si>
+    <t>Datos caja verde:</t>
+  </si>
+  <si>
+    <t>Datos caja naranja:</t>
+  </si>
+  <si>
+    <t>cantidad cartas rojas</t>
+  </si>
+  <si>
+    <t>cantidad cartas azules</t>
+  </si>
+  <si>
+    <t>Probabilidad</t>
+  </si>
+  <si>
+    <t>Evento</t>
+  </si>
+  <si>
+    <t>(E_1)</t>
+  </si>
+  <si>
+    <t>(E_2)</t>
+  </si>
+  <si>
+    <t>(E_3)</t>
+  </si>
+  <si>
+    <t>(R_1)</t>
+  </si>
+  <si>
+    <t>(R_2)</t>
+  </si>
+  <si>
+    <t>(R_3)</t>
+  </si>
+  <si>
+    <t>caja amarilla</t>
+  </si>
+  <si>
+    <t>caja verde</t>
+  </si>
+  <si>
+    <t>caja naranja</t>
+  </si>
+  <si>
+    <t>cantidad_rojas/cantidad_cartas</t>
+  </si>
+  <si>
+    <t>1/cantidad_cajas</t>
+  </si>
+  <si>
+    <t>3. Ley de probabilidad total (final)</t>
+  </si>
+  <si>
+    <t>2. Elegir una carta roja dada la elección de la caja P(R_i|E_i)</t>
+  </si>
+  <si>
+    <t>1. Elegir una caja P(E_i)</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>P(R)</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>4. Respuesta</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">La probabilidad de elegir una carta roja despues de elegir una caja es del </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.63%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -207,22 +308,24 @@
       <color theme="1"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -245,11 +348,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -276,9 +437,52 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -296,6 +500,648 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>32082</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>8022</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>40226</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>192505</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA8D3EB7-5581-A322-42B6-44C0DDA78848}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2582777" y="208548"/>
+          <a:ext cx="4925049" cy="1788694"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 198"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="76200" dist="38100" dir="7800000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="40000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="contrasting" dir="t">
+            <a:rot lat="0" lon="0" rev="4200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d prstMaterial="plastic">
+          <a:bevelT w="381000" h="114300" prst="relaxedInset"/>
+          <a:contourClr>
+            <a:srgbClr val="969696"/>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>98959</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>49477</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>242758</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>153388</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3" descr="Llave - Iconos gratis de señales">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B51DAB5-F77E-11E0-F6D7-F72E57CB00CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="32373" r="33813"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="10800000">
+          <a:off x="8095011" y="4225633"/>
+          <a:ext cx="143799" cy="499756"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>83125</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>48488</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>226924</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4" descr="Llave - Iconos gratis de señales">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9666FC4D-DEB5-43E3-9397-47B10AD96D99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="32373" r="33813"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="10800000">
+          <a:off x="8079177" y="2829293"/>
+          <a:ext cx="143799" cy="499756"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>199292</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>96692</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>68158</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>110209</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01C5FCD3-D16D-3BAD-8392-AEBB664B666F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11975123" y="2488200"/>
+          <a:ext cx="1320816" cy="417964"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="76200" dist="38100" dir="7800000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="40000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="contrasting" dir="t">
+            <a:rot lat="0" lon="0" rev="4200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d prstMaterial="plastic">
+          <a:bevelT w="381000" h="114300" prst="relaxedInset"/>
+          <a:contourClr>
+            <a:srgbClr val="969696"/>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>201648</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>191183</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>319156</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>15390</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagen 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4AC40D8-718E-4BA7-AF75-CB64BC82CD18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14269340" y="2582691"/>
+          <a:ext cx="3605124" cy="228654"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="76200" dist="38100" dir="7800000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="40000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="contrasting" dir="t">
+            <a:rot lat="0" lon="0" rev="4200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d prstMaterial="plastic">
+          <a:bevelT w="381000" h="114300" prst="relaxedInset"/>
+          <a:contourClr>
+            <a:srgbClr val="969696"/>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>197005</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>101473</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>97691</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104078</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Conector recto de flecha 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E533F6B-9B4F-FBEC-197A-75CBDF9D7859}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="16823473" y="3056546"/>
+          <a:ext cx="380189" cy="2605"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>441159</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>64169</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>96252</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>24064</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Abrir llave 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42C7EBCF-E0F9-4BEB-8C39-AE06C5BCC204}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2141622" y="2069432"/>
+          <a:ext cx="505325" cy="3184358"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 8333"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-GT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>376991</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>16043</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>32084</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>176464</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Abrir llave 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEFEA331-D6DA-48D5-A207-B72CA928A5E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7844591" y="2021306"/>
+          <a:ext cx="505325" cy="3184358"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 8333"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-GT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152292</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>116691</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1163267" cy="593239"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Rectángulo 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21DEA976-9B1C-EB83-35CB-42929C65326D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1002524" y="3734186"/>
+          <a:ext cx="1163267" cy="593239"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="2800" b="1" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Datos</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES" sz="3200" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>468111</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>116690</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2472728" cy="530658"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Rectángulo 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1B2896E-5006-4AA7-9FF8-50E3F3F66023}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6235248" y="3734185"/>
+          <a:ext cx="2472728" cy="530658"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="2800" b="1" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Procedimiento:</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -615,95 +1461,567 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5469043C-8A19-CE4F-A8A9-127F5C97849D}">
-  <dimension ref="B2:G10"/>
+  <dimension ref="C1:AF29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="171" zoomScaleNormal="171" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M12" zoomScale="116" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="29.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.8984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.796875" customWidth="1"/>
+    <col min="12" max="12" width="4.8984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.296875" customWidth="1"/>
+    <col min="19" max="19" width="6.5" customWidth="1"/>
+    <col min="20" max="20" width="4.296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="1.8984375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="1.8984375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="1.8984375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="1.8984375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="1.8984375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="1.8984375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.3984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="10"/>
-      <c r="C3" s="10" t="s">
+    <row r="1" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+    </row>
+    <row r="2" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+    </row>
+    <row r="3" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C3" s="29"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+    </row>
+    <row r="4" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C4" s="29"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+    </row>
+    <row r="5" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C5" s="29"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+    </row>
+    <row r="6" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C6" s="29"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+    </row>
+    <row r="7" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+    </row>
+    <row r="8" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+    </row>
+    <row r="9" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+    </row>
+    <row r="10" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+    </row>
+    <row r="11" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C11" s="29"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+    </row>
+    <row r="12" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C12" s="29"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+    </row>
+    <row r="14" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="D14" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="K14" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="S14" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="D15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="11">
+        <v>3</v>
+      </c>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="3:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D16" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="10"/>
-      <c r="C4" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="10"/>
-      <c r="C5" s="10" t="s">
+      <c r="E16" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+      <c r="F16" s="7">
+        <v>100</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="K16" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N16" s="14"/>
+    </row>
+    <row r="17" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="K17" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="L17" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="M17" s="22">
+        <f>1/$F$15</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N17" s="22"/>
+    </row>
+    <row r="18" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="D18" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="K18" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="M18" s="22">
+        <f t="shared" ref="M18:M19" si="0">1/$F$15</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N18" s="22"/>
+      <c r="P18" t="s">
+        <v>57</v>
+      </c>
+      <c r="T18" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="U18" t="s">
+        <v>37</v>
+      </c>
+      <c r="V18" s="25">
+        <f>M24</f>
+        <v>0.75</v>
+      </c>
+      <c r="W18" t="s">
+        <v>61</v>
+      </c>
+      <c r="X18" s="25">
+        <f>M17</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z18" s="25">
+        <f>M25</f>
+        <v>0.6</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB18" s="25">
+        <f>M18</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD18" s="25">
+        <f>M26</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF18" s="25">
+        <f>M19</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="19" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="D19" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="11">
+        <v>75</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="K19" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="M19" s="22">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N19" s="22"/>
+      <c r="T19" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="U19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="V19" s="28">
+        <f>(M24*M17)+(M25*M18)+(M26*M19)</f>
+        <v>0.6333333333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="D20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="11">
+        <v>25</v>
+      </c>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+    </row>
+    <row r="21" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="K21" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="S21" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="D22" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="4:32" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D23" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="11">
+        <v>60</v>
+      </c>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="K23" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N23" s="14"/>
+      <c r="T23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="D24" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="11">
+        <v>40</v>
+      </c>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="K24" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L24" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="M24" s="19">
+        <f>F19/F16</f>
+        <v>0.75</v>
+      </c>
+      <c r="N24" s="20"/>
+    </row>
+    <row r="25" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="K25" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L25" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="M25" s="21">
+        <f>F23/F16</f>
+        <v>0.6</v>
+      </c>
+      <c r="N25" s="18"/>
+      <c r="P25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="D26" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="K26" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="M26" s="21">
+        <f>F27/F16</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="N26" s="18"/>
+    </row>
+    <row r="27" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="D27" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="11">
+        <v>55</v>
+      </c>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+    </row>
+    <row r="28" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="D28" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="11">
+        <v>45</v>
+      </c>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+    </row>
+    <row r="29" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B10:G10"/>
+  <mergeCells count="11">
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="D12:M12"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K16:L16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -723,19 +2041,19 @@
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
@@ -748,7 +2066,7 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
@@ -756,7 +2074,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -774,17 +2092,17 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
@@ -795,23 +2113,23 @@
       <c r="C6" s="6"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="8">
         <v>0.2</v>
@@ -830,7 +2148,7 @@
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
       <c r="D8" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="8">
         <v>0.2</v>
@@ -849,7 +2167,7 @@
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="8">
         <v>0.6</v>
@@ -866,32 +2184,32 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -914,12 +2232,12 @@
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -948,7 +2266,7 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -1037,12 +2355,12 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D12" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D13" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1063,12 +2381,12 @@
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -1097,7 +2415,7 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -1190,7 +2508,7 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D12" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
@@ -1214,12 +2532,12 @@
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -1248,7 +2566,7 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -1309,26 +2627,26 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: finalización inciso 2
</commit_message>
<xml_diff>
--- a/labs/lab7/lab7.xlsx
+++ b/labs/lab7/lab7.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UVG GitHub Repositorios\2025\Inteligencia Artificial\labs\lab7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435D3F48-96ED-45CC-ADC4-8844F4224476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3AC487-8FE6-4BDF-BABC-62D7F112A80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8F1ECDA0-F4DF-3946-9953-220E6ED439C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8F1ECDA0-F4DF-3946-9953-220E6ED439C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Ej 1" sheetId="3" r:id="rId1"/>
-    <sheet name="Ej 2" sheetId="5" r:id="rId2"/>
+    <sheet name="Ej 2" sheetId="10" r:id="rId2"/>
     <sheet name="Ej 3" sheetId="4" r:id="rId3"/>
     <sheet name="Ej 4" sheetId="7" r:id="rId4"/>
     <sheet name="Ej 5" sheetId="8" r:id="rId5"/>
@@ -41,13 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
-  <si>
-    <t>Se tienen tres cajas, cada una conteniendo 100 cartas:</t>
-  </si>
-  <si>
-    <t>Se elige una de las cajas al azar, y luego se elige una carta dentro de la caja</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="62">
   <si>
     <t>enfermedad?</t>
   </si>
@@ -97,21 +91,6 @@
     <t>P(E3 | Si)</t>
   </si>
   <si>
-    <t>La caja Amarilla contiene 75 cartas rojas, y 25 cartas azules,</t>
-  </si>
-  <si>
-    <t>la caja Verde contiene 60 cartas rojas, y 40 cartas azules,</t>
-  </si>
-  <si>
-    <t>la caja Naranja contiene 55 cartas rojas, y 45 cartas azules.</t>
-  </si>
-  <si>
-    <t>seleccionada (sin ver la carta).</t>
-  </si>
-  <si>
-    <t>¿Cuál es la probabilidad de elegir una carta roja, si se sabe que a la persona le gusta mucho el color Amarillo?</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -238,30 +217,16 @@
     <t>4. Respuesta</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">La probabilidad de elegir una carta roja despues de elegir una caja es del </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0.63%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
+    <t>Color Favorito</t>
+  </si>
+  <si>
+    <t>La probabilidad de elegir una carta roja despues de elegir una caja es del</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Como el color amarillo es su favorito, asignamos una probabilidad mayor a 0.33 a la caja amarilla para reflejar su preferencia y en los demás colores se coloca un restante de probabilidad repartido en los colores equitativamente. Esto es modificable y podemos aumentarlo en las celdas a la izquierda. seleccionando el color de preferencia y su probabilidad.</t>
   </si>
 </sst>
 </file>
@@ -410,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -467,23 +432,40 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,7 +563,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>242758</xdr:colOff>
+      <xdr:colOff>250378</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>153388</xdr:rowOff>
     </xdr:to>
@@ -699,9 +681,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>68158</xdr:colOff>
+      <xdr:colOff>56728</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>110209</xdr:rowOff>
+      <xdr:rowOff>94969</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -766,8 +748,8 @@
       <xdr:rowOff>191183</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>319156</xdr:colOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>480641</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>15390</xdr:rowOff>
     </xdr:to>
@@ -1144,6 +1126,589 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>98959</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>49477</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>250378</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>153388</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2" descr="Llave - Iconos gratis de señales">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94D777A5-BE77-495C-9B57-5B9EF24F559B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="32373" r="33813"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="10800000">
+          <a:off x="12374779" y="4621477"/>
+          <a:ext cx="143799" cy="500151"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>199292</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>96692</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>56727</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>117536</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11391531-0895-4884-8158-9C139D1C23B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15363092" y="2870372"/>
+          <a:ext cx="1316666" cy="417377"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="76200" dist="38100" dir="7800000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="40000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="contrasting" dir="t">
+            <a:rot lat="0" lon="0" rev="4200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d prstMaterial="plastic">
+          <a:bevelT w="381000" h="114300" prst="relaxedInset"/>
+          <a:contourClr>
+            <a:srgbClr val="969696"/>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>201648</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>191183</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>400128</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>22717</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8846FD4F-0987-4AC4-B254-F50AA4EDB805}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17293308" y="2964863"/>
+          <a:ext cx="3599848" cy="228067"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="76200" dist="38100" dir="7800000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="40000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="contrasting" dir="t">
+            <a:rot lat="0" lon="0" rev="4200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d prstMaterial="plastic">
+          <a:bevelT w="381000" h="114300" prst="relaxedInset"/>
+          <a:contourClr>
+            <a:srgbClr val="969696"/>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>197005</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>101473</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>97691</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104078</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Conector recto de flecha 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C63CF97-6A54-4161-8004-B0FF885F3D6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="16808605" y="3073273"/>
+          <a:ext cx="380746" cy="2605"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>441159</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>64169</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>96252</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>24064</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Abrir llave 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{155C36F8-F91E-4FA8-877C-5D2C6DB7E918}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2148039" y="2441609"/>
+          <a:ext cx="508533" cy="3145055"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 8333"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-GT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>369371</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>16043</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>22559</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Abrir llave 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{422358F1-6B56-4249-9950-15BB11E45DAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8767936" y="2401434"/>
+          <a:ext cx="514580" cy="3777392"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 8333"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-GT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152292</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>116691</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1163267" cy="593239"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectángulo 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E945FE83-274C-4B6A-8419-966EF540EBDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1005732" y="3690471"/>
+          <a:ext cx="1163267" cy="593239"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="2800" b="1" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Datos</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES" sz="3200" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>468111</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>116690</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2472728" cy="530658"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectángulo 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65EC8177-9853-462C-AA34-FF757F5C3FCA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6251691" y="3690470"/>
+          <a:ext cx="2472728" cy="530658"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="2800" b="1" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Procedimiento:</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>25665</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1087683</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>193843</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Imagen 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63485627-3628-465F-8121-48E26E29B4E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2576360" y="190100"/>
+          <a:ext cx="7667956" cy="1808480"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 198"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="76200" dist="38100" dir="7800000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="40000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="contrasting" dir="t">
+            <a:rot lat="0" lon="0" rev="4200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d prstMaterial="plastic">
+          <a:bevelT w="381000" h="114300" prst="relaxedInset"/>
+          <a:contourClr>
+            <a:srgbClr val="969696"/>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -1461,10 +2026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5469043C-8A19-CE4F-A8A9-127F5C97849D}">
-  <dimension ref="C1:AF29"/>
+  <dimension ref="D2:AJ29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M12" zoomScale="116" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="Y20" sqref="Y20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AE10" sqref="AE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1489,218 +2054,92 @@
     <col min="30" max="30" width="4.3984375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="1.8984375" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="4.69921875" customWidth="1"/>
+    <col min="35" max="35" width="4.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-    </row>
-    <row r="2" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-    </row>
-    <row r="3" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-    </row>
-    <row r="4" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C4" s="29"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-    </row>
-    <row r="5" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C5" s="29"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-    </row>
-    <row r="6" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C6" s="29"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-    </row>
-    <row r="7" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C7" s="29"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-    </row>
-    <row r="8" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C8" s="29"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-    </row>
-    <row r="9" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C9" s="29"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-    </row>
-    <row r="10" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C10" s="29"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-    </row>
-    <row r="11" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C11" s="29"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-    </row>
-    <row r="12" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C12" s="29"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-    </row>
-    <row r="14" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+    </row>
+    <row r="14" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D14" s="10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E14" s="10"/>
       <c r="K14" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="S14" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="3:19" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D15" s="12" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F15" s="11">
         <v>3</v>
@@ -1709,12 +2148,12 @@
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
     </row>
-    <row r="16" spans="3:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D16" s="12" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F16" s="7">
         <v>100</v>
@@ -1722,102 +2161,102 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
-      <c r="K16" s="14" t="s">
+      <c r="K16" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="N16" s="27"/>
+    </row>
+    <row r="17" spans="4:36" x14ac:dyDescent="0.3">
+      <c r="K17" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="N16" s="14"/>
-    </row>
-    <row r="17" spans="4:32" x14ac:dyDescent="0.3">
-      <c r="K17" s="23" t="s">
-        <v>53</v>
-      </c>
       <c r="L17" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="M17" s="22">
+        <v>40</v>
+      </c>
+      <c r="M17" s="26">
         <f>1/$F$15</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="N17" s="22"/>
-    </row>
-    <row r="18" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="N17" s="26"/>
+    </row>
+    <row r="18" spans="4:36" x14ac:dyDescent="0.3">
       <c r="D18" s="10" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
-      <c r="K18" s="24" t="s">
-        <v>54</v>
+      <c r="K18" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="M18" s="22">
+        <v>41</v>
+      </c>
+      <c r="M18" s="26">
         <f t="shared" ref="M18:M19" si="0">1/$F$15</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="N18" s="22"/>
+      <c r="N18" s="26"/>
       <c r="P18" t="s">
-        <v>57</v>
-      </c>
-      <c r="T18" s="26" t="s">
-        <v>62</v>
+        <v>50</v>
+      </c>
+      <c r="T18" s="23" t="s">
+        <v>55</v>
       </c>
       <c r="U18" t="s">
-        <v>37</v>
-      </c>
-      <c r="V18" s="25">
+        <v>30</v>
+      </c>
+      <c r="V18" s="23">
         <f>M24</f>
         <v>0.75</v>
       </c>
       <c r="W18" t="s">
-        <v>61</v>
-      </c>
-      <c r="X18" s="25">
+        <v>54</v>
+      </c>
+      <c r="X18" s="23">
         <f>M17</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="Y18" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z18" s="25">
+        <v>56</v>
+      </c>
+      <c r="Z18" s="23">
         <f>M25</f>
         <v>0.6</v>
       </c>
       <c r="AA18" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB18" s="25">
+        <v>54</v>
+      </c>
+      <c r="AB18" s="23">
         <f>M18</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="AC18" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD18" s="25">
+        <v>56</v>
+      </c>
+      <c r="AD18" s="23">
         <f>M26</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="AE18" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF18" s="25">
+        <v>54</v>
+      </c>
+      <c r="AF18" s="23">
         <f>M19</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="19" spans="4:32" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:36" x14ac:dyDescent="0.3">
       <c r="D19" s="12" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F19" s="11">
         <v>75</v>
@@ -1825,34 +2264,34 @@
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
-      <c r="K19" s="24" t="s">
-        <v>55</v>
+      <c r="K19" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="M19" s="22">
+        <v>42</v>
+      </c>
+      <c r="M19" s="26">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="N19" s="22"/>
-      <c r="T19" s="27" t="s">
-        <v>62</v>
+      <c r="N19" s="26"/>
+      <c r="T19" s="24" t="s">
+        <v>55</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="V19" s="28">
+        <v>30</v>
+      </c>
+      <c r="V19" s="24">
         <f>(M24*M17)+(M25*M18)+(M26*M19)</f>
         <v>0.6333333333333333</v>
       </c>
     </row>
-    <row r="20" spans="4:32" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:36" x14ac:dyDescent="0.3">
       <c r="D20" s="12" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F20" s="11">
         <v>25</v>
@@ -1861,33 +2300,33 @@
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="4:32" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:36" x14ac:dyDescent="0.3">
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="K21" s="17" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="S21" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="4:32" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="4:36" x14ac:dyDescent="0.3">
       <c r="D22" s="10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="4:32" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:36" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D23" s="12" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E23" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F23" s="11">
         <v>60</v>
@@ -1895,24 +2334,45 @@
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
-      <c r="K23" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="N23" s="14"/>
-      <c r="T23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="K23" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="N23" s="27"/>
+      <c r="T23" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="U23" s="32"/>
+      <c r="V23" s="32"/>
+      <c r="W23" s="32"/>
+      <c r="X23" s="32"/>
+      <c r="Y23" s="32"/>
+      <c r="Z23" s="32"/>
+      <c r="AA23" s="32"/>
+      <c r="AB23" s="32"/>
+      <c r="AC23" s="32"/>
+      <c r="AD23" s="32"/>
+      <c r="AE23" s="32"/>
+      <c r="AF23" s="32"/>
+      <c r="AG23" s="32"/>
+      <c r="AH23" s="32"/>
+      <c r="AI23" s="33">
+        <f>V19</f>
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="4:36" x14ac:dyDescent="0.3">
       <c r="D24" s="12" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F24" s="11">
         <v>40</v>
@@ -1921,63 +2381,63 @@
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="K24" s="13" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="L24" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="M24" s="19">
+        <v>43</v>
+      </c>
+      <c r="M24" s="29">
         <f>F19/F16</f>
         <v>0.75</v>
       </c>
-      <c r="N24" s="20"/>
-    </row>
-    <row r="25" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="N24" s="30"/>
+    </row>
+    <row r="25" spans="4:36" x14ac:dyDescent="0.3">
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
       <c r="K25" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="L25" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="M25" s="21">
+        <v>44</v>
+      </c>
+      <c r="M25" s="25">
         <f>F23/F16</f>
         <v>0.6</v>
       </c>
-      <c r="N25" s="18"/>
+      <c r="N25" s="26"/>
       <c r="P25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="4:32" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="4:36" x14ac:dyDescent="0.3">
       <c r="D26" s="10" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
       <c r="K26" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="L26" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="M26" s="21">
+        <v>45</v>
+      </c>
+      <c r="M26" s="25">
         <f>F27/F16</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="N26" s="18"/>
-    </row>
-    <row r="27" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="N26" s="26"/>
+    </row>
+    <row r="27" spans="4:36" x14ac:dyDescent="0.3">
       <c r="D27" s="12" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E27" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F27" s="11">
         <v>55</v>
@@ -1986,12 +2446,12 @@
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="4:32" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:36" x14ac:dyDescent="0.3">
       <c r="D28" s="12" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E28" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F28" s="11">
         <v>45</v>
@@ -2000,25 +2460,26 @@
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
     </row>
-    <row r="29" spans="4:32" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:36" x14ac:dyDescent="0.3">
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M23:N23"/>
+  <mergeCells count="12">
+    <mergeCell ref="T23:AH23"/>
     <mergeCell ref="D12:M12"/>
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="M25:N25"/>
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M23:N23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2026,59 +2487,502 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0895F84E-B49B-A446-B58F-A023063A27C9}">
-  <dimension ref="B2:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F314B675-4816-470D-A6FF-401765C6766D}">
+  <dimension ref="D2:AK30"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="29.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.8984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.796875" customWidth="1"/>
+    <col min="12" max="12" width="4.8984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.296875" customWidth="1"/>
+    <col min="17" max="17" width="15.09765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.5" customWidth="1"/>
+    <col min="21" max="21" width="4.296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="1.8984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="1.8984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="1.8984375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="1.8984375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="1.8984375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="1.8984375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.69921875" customWidth="1"/>
+    <col min="36" max="36" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="1.3984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
-        <v>22</v>
-      </c>
+    <row r="2" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+    </row>
+    <row r="14" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="K14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="T14" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D15" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="11">
+        <v>3</v>
+      </c>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="4:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="7">
+        <v>100</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="K16" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+    </row>
+    <row r="17" spans="4:37" x14ac:dyDescent="0.3">
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
+    </row>
+    <row r="18" spans="4:37" x14ac:dyDescent="0.3">
+      <c r="D18" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="34"/>
+      <c r="U18" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="V18" t="s">
+        <v>30</v>
+      </c>
+      <c r="W18" s="23">
+        <f>M28</f>
+        <v>0.75</v>
+      </c>
+      <c r="X18" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y18" s="23">
+        <f>M21</f>
+        <v>0.8</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA18" s="23">
+        <f>M29</f>
+        <v>0.6</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC18" s="23">
+        <f>M22</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE18" s="23">
+        <f>M30</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG18" s="23">
+        <f>M23</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="4:37" x14ac:dyDescent="0.3">
+      <c r="D19" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="11">
+        <v>75</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="U19" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="V19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="W19" s="24">
+        <f>(M28*M21)+(M29*M22)+(M30*M23)</f>
+        <v>0.71500000000000008</v>
+      </c>
+    </row>
+    <row r="20" spans="4:37" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="11">
+        <v>25</v>
+      </c>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="K20" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="N20" s="27"/>
+      <c r="Q20" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="R20" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="4:37" x14ac:dyDescent="0.3">
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="K21" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="M21" s="18">
+        <f>IF(K21=$Q$21,$R$21,(1-$R$21)/2)</f>
+        <v>0.8</v>
+      </c>
+      <c r="N21" s="18"/>
+      <c r="Q21" t="s">
+        <v>46</v>
+      </c>
+      <c r="R21">
+        <v>0.8</v>
+      </c>
+      <c r="T21" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="4:37" x14ac:dyDescent="0.3">
+      <c r="D22" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="K22" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="M22" s="18">
+        <f>IF(K22=$Q$21,$R$21,(1-$R$21)/2)</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="N22" s="18"/>
+    </row>
+    <row r="23" spans="4:37" x14ac:dyDescent="0.3">
+      <c r="D23" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="11">
+        <v>60</v>
+      </c>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="K23" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="M23" s="18">
+        <f>IF(K23=$Q$21,$R$21,(1-$R$21)/2)</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="N23" s="18"/>
+      <c r="U23" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="V23" s="32"/>
+      <c r="W23" s="32"/>
+      <c r="X23" s="32"/>
+      <c r="Y23" s="32"/>
+      <c r="Z23" s="32"/>
+      <c r="AA23" s="32"/>
+      <c r="AB23" s="32"/>
+      <c r="AC23" s="32"/>
+      <c r="AD23" s="32"/>
+      <c r="AE23" s="32"/>
+      <c r="AF23" s="32"/>
+      <c r="AG23" s="32"/>
+      <c r="AH23" s="32"/>
+      <c r="AI23" s="32"/>
+      <c r="AJ23" s="24">
+        <f>W19</f>
+        <v>0.71500000000000008</v>
+      </c>
+      <c r="AK23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="4:37" x14ac:dyDescent="0.3">
+      <c r="D24" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="11">
+        <v>40</v>
+      </c>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+    </row>
+    <row r="25" spans="4:37" x14ac:dyDescent="0.3">
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="K25" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="4:37" x14ac:dyDescent="0.3">
+      <c r="D26" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+    </row>
+    <row r="27" spans="4:37" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D27" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="11">
+        <v>55</v>
+      </c>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="K27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="N27" s="14"/>
+    </row>
+    <row r="28" spans="4:37" x14ac:dyDescent="0.3">
+      <c r="D28" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="11">
+        <v>45</v>
+      </c>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="K28" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="L28" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="M28" s="19">
+        <f>F19/F16</f>
+        <v>0.75</v>
+      </c>
+      <c r="N28" s="20"/>
+    </row>
+    <row r="29" spans="4:37" x14ac:dyDescent="0.3">
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="K29" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="L29" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="M29" s="21">
+        <f>F23/F16</f>
+        <v>0.6</v>
+      </c>
+      <c r="N29" s="31"/>
+      <c r="P29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="4:37" x14ac:dyDescent="0.3">
+      <c r="K30" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="L30" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="M30" s="21">
+        <f>F27/F16</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="N30" s="31"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="U23:AI23"/>
+    <mergeCell ref="K16:R18"/>
+    <mergeCell ref="D12:M12"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:N20"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q21" xr:uid="{839C76A6-EB4B-4419-9C09-473E969262AD}">
+      <formula1>$K$21:$K$23</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2092,17 +2996,17 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
@@ -2113,23 +3017,23 @@
       <c r="C6" s="6"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7" s="8">
         <v>0.2</v>
@@ -2148,7 +3052,7 @@
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
       <c r="D8" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E8" s="8">
         <v>0.2</v>
@@ -2167,7 +3071,7 @@
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="8">
         <v>0.6</v>
@@ -2184,32 +3088,32 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2232,12 +3136,12 @@
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -2266,7 +3170,7 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -2355,12 +3259,12 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D12" s="7" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D13" s="7" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2381,12 +3285,12 @@
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -2415,7 +3319,7 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -2508,7 +3412,7 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D12" s="7" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
@@ -2532,12 +3436,12 @@
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -2566,7 +3470,7 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -2627,26 +3531,26 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: finalización inciso, cambio de respuesta
</commit_message>
<xml_diff>
--- a/labs/lab7/lab7.xlsx
+++ b/labs/lab7/lab7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UVG GitHub Repositorios\2025\Inteligencia Artificial\labs\lab7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3AC487-8FE6-4BDF-BABC-62D7F112A80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F6761F-E071-4D8C-B013-05AF227560BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8F1ECDA0-F4DF-3946-9953-220E6ED439C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{8F1ECDA0-F4DF-3946-9953-220E6ED439C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Ej 1" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="65">
   <si>
     <t>enfermedad?</t>
   </si>
@@ -227,6 +227,15 @@
   </si>
   <si>
     <t>Como el color amarillo es su favorito, asignamos una probabilidad mayor a 0.33 a la caja amarilla para reflejar su preferencia y en los demás colores se coloca un restante de probabilidad repartido en los colores equitativamente. Esto es modificable y podemos aumentarlo en las celdas a la izquierda. seleccionando el color de preferencia y su probabilidad.</t>
+  </si>
+  <si>
+    <t>La probabilidad de elegir una carta roja despues de elegir una</t>
+  </si>
+  <si>
+    <t>(con probabilidad de elección de</t>
+  </si>
+  <si>
+    <t>) es</t>
   </si>
 </sst>
 </file>
@@ -437,17 +446,17 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -455,17 +464,17 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1263,8 +1272,8 @@
       <xdr:rowOff>191183</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>400128</xdr:colOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>675852</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>22717</xdr:rowOff>
     </xdr:to>
@@ -2028,41 +2037,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5469043C-8A19-CE4F-A8A9-127F5C97849D}">
   <dimension ref="D2:AJ29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AE10" sqref="AE10"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="29.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.8984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.796875" customWidth="1"/>
-    <col min="12" max="12" width="4.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.75" customWidth="1"/>
+    <col min="12" max="12" width="4.875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.296875" customWidth="1"/>
+    <col min="15" max="15" width="4.25" customWidth="1"/>
     <col min="19" max="19" width="6.5" customWidth="1"/>
-    <col min="20" max="20" width="4.296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="1.8984375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="1.8984375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="1.8984375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="1.8984375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="1.8984375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="1.8984375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4.69921875" customWidth="1"/>
+    <col min="20" max="20" width="4.25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="4.75" customWidth="1"/>
     <col min="35" max="35" width="4.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="4:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -2070,7 +2079,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="4:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -2078,7 +2087,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="4:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -2086,43 +2095,43 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="4:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="4:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="4:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="4:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="4:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="4:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-    </row>
-    <row r="14" spans="4:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+    </row>
+    <row r="14" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D14" s="10" t="s">
         <v>32</v>
       </c>
@@ -2134,7 +2143,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="4:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D15" s="12" t="s">
         <v>29</v>
       </c>
@@ -2148,7 +2157,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
     </row>
-    <row r="16" spans="4:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="12" t="s">
         <v>31</v>
       </c>
@@ -2161,29 +2170,29 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
-      <c r="K16" s="27" t="s">
+      <c r="K16" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27" t="s">
+      <c r="L16" s="32"/>
+      <c r="M16" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="N16" s="27"/>
-    </row>
-    <row r="17" spans="4:36" x14ac:dyDescent="0.3">
+      <c r="N16" s="32"/>
+    </row>
+    <row r="17" spans="4:36" x14ac:dyDescent="0.25">
       <c r="K17" s="22" t="s">
         <v>46</v>
       </c>
       <c r="L17" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="M17" s="26">
+      <c r="M17" s="28">
         <f>1/$F$15</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="N17" s="26"/>
-    </row>
-    <row r="18" spans="4:36" x14ac:dyDescent="0.3">
+      <c r="N17" s="28"/>
+    </row>
+    <row r="18" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D18" s="10" t="s">
         <v>33</v>
       </c>
@@ -2197,11 +2206,11 @@
       <c r="L18" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="M18" s="26">
+      <c r="M18" s="28">
         <f t="shared" ref="M18:M19" si="0">1/$F$15</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="N18" s="26"/>
+      <c r="N18" s="28"/>
       <c r="P18" t="s">
         <v>50</v>
       </c>
@@ -2251,7 +2260,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="19" spans="4:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D19" s="12" t="s">
         <v>36</v>
       </c>
@@ -2270,11 +2279,11 @@
       <c r="L19" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="M19" s="26">
+      <c r="M19" s="28">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="N19" s="26"/>
+      <c r="N19" s="28"/>
       <c r="T19" s="24" t="s">
         <v>55</v>
       </c>
@@ -2286,7 +2295,7 @@
         <v>0.6333333333333333</v>
       </c>
     </row>
-    <row r="20" spans="4:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D20" s="12" t="s">
         <v>37</v>
       </c>
@@ -2300,7 +2309,7 @@
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="4:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:36" x14ac:dyDescent="0.25">
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -2312,7 +2321,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="4:36" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D22" s="10" t="s">
         <v>34</v>
       </c>
@@ -2321,7 +2330,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="4:36" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D23" s="12" t="s">
         <v>36</v>
       </c>
@@ -2334,32 +2343,32 @@
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
-      <c r="K23" s="27" t="s">
+      <c r="K23" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27" t="s">
+      <c r="L23" s="32"/>
+      <c r="M23" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="N23" s="27"/>
-      <c r="T23" s="32" t="s">
+      <c r="N23" s="32"/>
+      <c r="T23" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="U23" s="32"/>
-      <c r="V23" s="32"/>
-      <c r="W23" s="32"/>
-      <c r="X23" s="32"/>
-      <c r="Y23" s="32"/>
-      <c r="Z23" s="32"/>
-      <c r="AA23" s="32"/>
-      <c r="AB23" s="32"/>
-      <c r="AC23" s="32"/>
-      <c r="AD23" s="32"/>
-      <c r="AE23" s="32"/>
-      <c r="AF23" s="32"/>
-      <c r="AG23" s="32"/>
-      <c r="AH23" s="32"/>
-      <c r="AI23" s="33">
+      <c r="U23" s="26"/>
+      <c r="V23" s="26"/>
+      <c r="W23" s="26"/>
+      <c r="X23" s="26"/>
+      <c r="Y23" s="26"/>
+      <c r="Z23" s="26"/>
+      <c r="AA23" s="26"/>
+      <c r="AB23" s="26"/>
+      <c r="AC23" s="26"/>
+      <c r="AD23" s="26"/>
+      <c r="AE23" s="26"/>
+      <c r="AF23" s="26"/>
+      <c r="AG23" s="26"/>
+      <c r="AH23" s="26"/>
+      <c r="AI23" s="25">
         <f>V19</f>
         <v>0.6333333333333333</v>
       </c>
@@ -2367,7 +2376,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="4:36" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D24" s="12" t="s">
         <v>37</v>
       </c>
@@ -2392,7 +2401,7 @@
       </c>
       <c r="N24" s="30"/>
     </row>
-    <row r="25" spans="4:36" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:36" x14ac:dyDescent="0.25">
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -2403,16 +2412,16 @@
       <c r="L25" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="M25" s="25">
+      <c r="M25" s="31">
         <f>F23/F16</f>
         <v>0.6</v>
       </c>
-      <c r="N25" s="26"/>
+      <c r="N25" s="28"/>
       <c r="P25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="4:36" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D26" s="10" t="s">
         <v>35</v>
       </c>
@@ -2426,13 +2435,13 @@
       <c r="L26" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="M26" s="25">
+      <c r="M26" s="31">
         <f>F27/F16</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="N26" s="26"/>
-    </row>
-    <row r="27" spans="4:36" x14ac:dyDescent="0.3">
+      <c r="N26" s="28"/>
+    </row>
+    <row r="27" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D27" s="12" t="s">
         <v>36</v>
       </c>
@@ -2446,7 +2455,7 @@
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="4:36" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D28" s="12" t="s">
         <v>37</v>
       </c>
@@ -2460,7 +2469,7 @@
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
     </row>
-    <row r="29" spans="4:36" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:36" x14ac:dyDescent="0.25">
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
@@ -2468,6 +2477,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M23:N23"/>
     <mergeCell ref="T23:AH23"/>
     <mergeCell ref="D12:M12"/>
     <mergeCell ref="M18:N18"/>
@@ -2475,11 +2489,6 @@
     <mergeCell ref="M25:N25"/>
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M23:N23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2488,45 +2497,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F314B675-4816-470D-A6FF-401765C6766D}">
-  <dimension ref="D2:AK30"/>
+  <dimension ref="D2:AN30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="29.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.8984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.796875" customWidth="1"/>
-    <col min="12" max="12" width="4.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.75" customWidth="1"/>
+    <col min="12" max="12" width="4.875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.296875" customWidth="1"/>
-    <col min="17" max="17" width="15.09765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.25" customWidth="1"/>
+    <col min="17" max="17" width="15.125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6.5" customWidth="1"/>
-    <col min="21" max="21" width="4.296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="1.8984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="1.8984375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="1.8984375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="1.8984375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="1.8984375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="1.8984375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="4.69921875" customWidth="1"/>
-    <col min="36" max="36" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="1.3984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.25" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.375" customWidth="1"/>
+    <col min="35" max="35" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="26.375" customWidth="1"/>
+    <col min="37" max="37" width="4.375" customWidth="1"/>
+    <col min="38" max="38" width="3.75" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="4.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -2534,7 +2546,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -2542,7 +2554,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -2550,43 +2562,43 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="4:20" x14ac:dyDescent="0.3">
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-    </row>
-    <row r="14" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+    </row>
+    <row r="14" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D14" s="10" t="s">
         <v>32</v>
       </c>
@@ -2598,7 +2610,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D15" s="12" t="s">
         <v>29</v>
       </c>
@@ -2612,7 +2624,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
     </row>
-    <row r="16" spans="4:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16" s="12" t="s">
         <v>31</v>
       </c>
@@ -2625,28 +2637,28 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
-      <c r="K16" s="34" t="s">
+      <c r="K16" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="34"/>
-      <c r="R16" s="34"/>
-    </row>
-    <row r="17" spans="4:37" x14ac:dyDescent="0.3">
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="34"/>
-      <c r="P17" s="34"/>
-      <c r="Q17" s="34"/>
-      <c r="R17" s="34"/>
-    </row>
-    <row r="18" spans="4:37" x14ac:dyDescent="0.3">
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="33"/>
+    </row>
+    <row r="17" spans="4:40" x14ac:dyDescent="0.25">
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="33"/>
+    </row>
+    <row r="18" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D18" s="10" t="s">
         <v>33</v>
       </c>
@@ -2654,14 +2666,14 @@
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="34"/>
-      <c r="R18" s="34"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
       <c r="U18" s="23" t="s">
         <v>55</v>
       </c>
@@ -2708,7 +2720,7 @@
         <v>9.9999999999999978E-2</v>
       </c>
     </row>
-    <row r="19" spans="4:37" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D19" s="12" t="s">
         <v>36</v>
       </c>
@@ -2732,7 +2744,7 @@
         <v>0.71500000000000008</v>
       </c>
     </row>
-    <row r="20" spans="4:37" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:40" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="12" t="s">
         <v>37</v>
       </c>
@@ -2745,14 +2757,14 @@
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
-      <c r="K20" s="27" t="s">
+      <c r="K20" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27" t="s">
+      <c r="L20" s="32"/>
+      <c r="M20" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="N20" s="27"/>
+      <c r="N20" s="32"/>
       <c r="Q20" s="10" t="s">
         <v>58</v>
       </c>
@@ -2760,7 +2772,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="4:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:40" x14ac:dyDescent="0.25">
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -2786,7 +2798,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="4:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D22" s="10" t="s">
         <v>34</v>
       </c>
@@ -2806,7 +2818,7 @@
       </c>
       <c r="N22" s="18"/>
     </row>
-    <row r="23" spans="4:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D23" s="12" t="s">
         <v>36</v>
       </c>
@@ -2830,32 +2842,45 @@
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="N23" s="18"/>
-      <c r="U23" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="V23" s="32"/>
-      <c r="W23" s="32"/>
-      <c r="X23" s="32"/>
-      <c r="Y23" s="32"/>
-      <c r="Z23" s="32"/>
-      <c r="AA23" s="32"/>
-      <c r="AB23" s="32"/>
-      <c r="AC23" s="32"/>
-      <c r="AD23" s="32"/>
-      <c r="AE23" s="32"/>
-      <c r="AF23" s="32"/>
-      <c r="AG23" s="32"/>
-      <c r="AH23" s="32"/>
-      <c r="AI23" s="32"/>
-      <c r="AJ23" s="24">
+      <c r="U23" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="V23" s="34"/>
+      <c r="W23" s="34"/>
+      <c r="X23" s="34"/>
+      <c r="Y23" s="34"/>
+      <c r="Z23" s="34"/>
+      <c r="AA23" s="34"/>
+      <c r="AB23" s="34"/>
+      <c r="AC23" s="34"/>
+      <c r="AD23" s="34"/>
+      <c r="AE23" s="34"/>
+      <c r="AF23" s="34"/>
+      <c r="AG23" s="34"/>
+      <c r="AH23" s="34"/>
+      <c r="AI23" s="17" t="str">
+        <f>Q21</f>
+        <v>caja amarilla</v>
+      </c>
+      <c r="AJ23" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK23" s="17">
+        <f>R21</f>
+        <v>0.8</v>
+      </c>
+      <c r="AL23" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM23" s="24">
         <f>W19</f>
         <v>0.71500000000000008</v>
       </c>
-      <c r="AK23" t="s">
+      <c r="AN23" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="4:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D24" s="12" t="s">
         <v>37</v>
       </c>
@@ -2869,7 +2894,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="4:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:40" x14ac:dyDescent="0.25">
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -2878,7 +2903,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="4:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D26" s="10" t="s">
         <v>35</v>
       </c>
@@ -2887,7 +2912,7 @@
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="4:37" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:40" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="12" t="s">
         <v>36</v>
       </c>
@@ -2909,7 +2934,7 @@
       </c>
       <c r="N27" s="14"/>
     </row>
-    <row r="28" spans="4:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D28" s="12" t="s">
         <v>37</v>
       </c>
@@ -2934,7 +2959,7 @@
       </c>
       <c r="N28" s="20"/>
     </row>
-    <row r="29" spans="4:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:40" x14ac:dyDescent="0.25">
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
@@ -2949,12 +2974,12 @@
         <f>F23/F16</f>
         <v>0.6</v>
       </c>
-      <c r="N29" s="31"/>
+      <c r="N29" s="18"/>
       <c r="P29" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="4:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:40" x14ac:dyDescent="0.25">
       <c r="K30" s="13" t="s">
         <v>48</v>
       </c>
@@ -2965,15 +2990,15 @@
         <f>F27/F16</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="N30" s="31"/>
+      <c r="N30" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="U23:AI23"/>
     <mergeCell ref="K16:R18"/>
     <mergeCell ref="D12:M12"/>
     <mergeCell ref="K20:L20"/>
     <mergeCell ref="M20:N20"/>
+    <mergeCell ref="U23:AH23"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q21" xr:uid="{839C76A6-EB4B-4419-9C09-473E969262AD}">
@@ -2992,27 +3017,27 @@
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
       <c r="D6" s="8"/>
@@ -3029,7 +3054,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="9" t="s">
@@ -3048,7 +3073,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
       <c r="D8" s="9" t="s">
@@ -3067,7 +3092,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="9" t="s">
@@ -3086,32 +3111,32 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>1</v>
       </c>
@@ -3129,17 +3154,17 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="5.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="5.796875" style="1"/>
+    <col min="1" max="16384" width="5.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
@@ -3149,7 +3174,7 @@
       <c r="M4" s="4"/>
       <c r="O4" s="4"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D5" s="1">
         <v>1</v>
       </c>
@@ -3168,7 +3193,7 @@
       <c r="M5" s="4"/>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -3193,7 +3218,7 @@
       <c r="M6" s="4"/>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <v>2</v>
       </c>
@@ -3215,7 +3240,7 @@
       <c r="M7" s="4"/>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <v>3</v>
       </c>
@@ -3232,7 +3257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <v>4</v>
       </c>
@@ -3254,15 +3279,15 @@
       <c r="M9" s="4"/>
       <c r="O9" s="4"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D12" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D13" s="7" t="s">
         <v>20</v>
       </c>
@@ -3278,17 +3303,17 @@
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="5.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="5.796875" style="1"/>
+    <col min="1" max="16384" width="5.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
@@ -3298,7 +3323,7 @@
       <c r="M4" s="4"/>
       <c r="O4" s="4"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D5" s="1">
         <v>1</v>
       </c>
@@ -3317,7 +3342,7 @@
       <c r="M5" s="4"/>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -3342,7 +3367,7 @@
       <c r="M6" s="4"/>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <v>2</v>
       </c>
@@ -3364,7 +3389,7 @@
       <c r="M7" s="4"/>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <v>3</v>
       </c>
@@ -3381,7 +3406,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <v>4</v>
       </c>
@@ -3404,18 +3429,18 @@
       <c r="M9" s="4"/>
       <c r="O9" s="4"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D12" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D13" s="7"/>
     </row>
   </sheetData>
@@ -3429,17 +3454,17 @@
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="5.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="5.796875" style="1"/>
+    <col min="1" max="16384" width="5.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
@@ -3449,7 +3474,7 @@
       <c r="M4" s="4"/>
       <c r="O4" s="4"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D5" s="1">
         <v>1</v>
       </c>
@@ -3468,7 +3493,7 @@
       <c r="M5" s="4"/>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -3485,7 +3510,7 @@
       <c r="M6" s="4"/>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <v>2</v>
       </c>
@@ -3499,7 +3524,7 @@
       <c r="M7" s="4"/>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <v>3</v>
       </c>
@@ -3508,7 +3533,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <v>4</v>
       </c>
@@ -3523,13 +3548,13 @@
       <c r="M9" s="4"/>
       <c r="O9" s="4"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
@@ -3537,7 +3562,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>25</v>
       </c>
@@ -3545,7 +3570,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>

</xml_diff>